<commit_message>
Add metrics to new and old synonyms; Fix q2 metrics
</commit_message>
<xml_diff>
--- a/solr/solrMetrics/q2/q2Metrics.xlsx
+++ b/solr/solrMetrics/q2/q2Metrics.xlsx
@@ -294,7 +294,7 @@
 </styleSheet>
 </file>
 
-<file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart5.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
@@ -438,36 +438,6 @@
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="10"/>
-                <c:pt idx="0">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>0</c:v>
-                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
@@ -574,33 +544,6 @@
                 <c:pt idx="0">
                   <c:v>1</c:v>
                 </c:pt>
-                <c:pt idx="1">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>0</c:v>
-                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
@@ -708,31 +651,16 @@
                   <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.5</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.333333333333333</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0</c:v>
+                  <c:v>0.75</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>0</c:v>
+                  <c:v>0.6</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -747,11 +675,11 @@
           </c:spPr>
         </c:hiLowLines>
         <c:marker val="0"/>
-        <c:axId val="25887848"/>
-        <c:axId val="19547453"/>
+        <c:axId val="6807767"/>
+        <c:axId val="65413307"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="25887848"/>
+        <c:axId val="6807767"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -812,7 +740,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="19547453"/>
+        <c:crossAx val="65413307"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -820,7 +748,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="19547453"/>
+        <c:axId val="65413307"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -891,7 +819,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="25887848"/>
+        <c:crossAx val="6807767"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -944,7 +872,7 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart6.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
@@ -1382,25 +1310,25 @@
                   <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0.5</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>0.5</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>0.5</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>0.333333333333333</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>0.333333333333333</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>0.333333333333333</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>0.333333333333333</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1415,11 +1343,11 @@
           </c:spPr>
         </c:hiLowLines>
         <c:marker val="0"/>
-        <c:axId val="83760539"/>
-        <c:axId val="51610477"/>
+        <c:axId val="36929984"/>
+        <c:axId val="78329878"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="83760539"/>
+        <c:axId val="36929984"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1488,7 +1416,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="51610477"/>
+        <c:crossAx val="78329878"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1496,7 +1424,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="51610477"/>
+        <c:axId val="78329878"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1539,7 +1467,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="83760539"/>
+        <c:crossAx val="36929984"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1592,7 +1520,7 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart7.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
@@ -1741,11 +1669,11 @@
           </c:spPr>
         </c:hiLowLines>
         <c:marker val="0"/>
-        <c:axId val="73892562"/>
-        <c:axId val="30326501"/>
+        <c:axId val="80334322"/>
+        <c:axId val="18610057"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="73892562"/>
+        <c:axId val="80334322"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1814,7 +1742,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="30326501"/>
+        <c:crossAx val="18610057"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1822,7 +1750,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="30326501"/>
+        <c:axId val="18610057"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1901,7 +1829,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="73892562"/>
+        <c:crossAx val="80334322"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1954,7 +1882,7 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart8.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
@@ -2135,11 +2063,11 @@
           </c:spPr>
         </c:hiLowLines>
         <c:marker val="0"/>
-        <c:axId val="36114492"/>
-        <c:axId val="30226140"/>
+        <c:axId val="71905639"/>
+        <c:axId val="21640911"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="36114492"/>
+        <c:axId val="71905639"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2208,7 +2136,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="30226140"/>
+        <c:crossAx val="21640911"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -2216,7 +2144,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="30226140"/>
+        <c:axId val="21640911"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2295,7 +2223,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="36114492"/>
+        <c:crossAx val="71905639"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -2359,9 +2287,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>10</xdr:col>
-      <xdr:colOff>632880</xdr:colOff>
+      <xdr:colOff>632520</xdr:colOff>
       <xdr:row>42</xdr:row>
-      <xdr:rowOff>171000</xdr:rowOff>
+      <xdr:rowOff>170640</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
@@ -2370,7 +2298,7 @@
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
         <a:off x="1440000" y="4924440"/>
-        <a:ext cx="5108400" cy="3152160"/>
+        <a:ext cx="5108040" cy="3151800"/>
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
@@ -2389,9 +2317,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>18</xdr:col>
-      <xdr:colOff>428040</xdr:colOff>
+      <xdr:colOff>427680</xdr:colOff>
       <xdr:row>42</xdr:row>
-      <xdr:rowOff>104040</xdr:rowOff>
+      <xdr:rowOff>103680</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
@@ -2400,7 +2328,7 @@
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
         <a:off x="7053480" y="4857480"/>
-        <a:ext cx="5111280" cy="3152160"/>
+        <a:ext cx="5116680" cy="3151800"/>
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
@@ -2424,9 +2352,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>13</xdr:col>
-      <xdr:colOff>793080</xdr:colOff>
+      <xdr:colOff>792720</xdr:colOff>
       <xdr:row>26</xdr:row>
-      <xdr:rowOff>189720</xdr:rowOff>
+      <xdr:rowOff>189360</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
@@ -2434,8 +2362,8 @@
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
-        <a:off x="4647240" y="2724120"/>
-        <a:ext cx="4357080" cy="2666160"/>
+        <a:off x="4648320" y="2724120"/>
+        <a:ext cx="4361760" cy="2665800"/>
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
@@ -2454,9 +2382,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>8</xdr:col>
-      <xdr:colOff>801720</xdr:colOff>
+      <xdr:colOff>801360</xdr:colOff>
       <xdr:row>26</xdr:row>
-      <xdr:rowOff>189720</xdr:rowOff>
+      <xdr:rowOff>189360</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
@@ -2465,7 +2393,7 @@
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
         <a:off x="200160" y="2724120"/>
-        <a:ext cx="4352040" cy="2666160"/>
+        <a:ext cx="4351680" cy="2665800"/>
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
@@ -2486,10 +2414,10 @@
   <dimension ref="A1:Q25"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
+      <selection pane="topLeft" activeCell="L20" activeCellId="0" sqref="L20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.66015625" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="12.6796875" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="5.5"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="2" style="0" width="9.51"/>
@@ -2572,10 +2500,7 @@
       <c r="D4" s="4" t="n">
         <v>1</v>
       </c>
-      <c r="F4" s="5" t="n">
-        <f aca="false">SUM(B4)/A4</f>
-        <v>0</v>
-      </c>
+      <c r="F4" s="5"/>
       <c r="G4" s="5" t="n">
         <f aca="false">SUM(C4)/A4</f>
         <v>1</v>
@@ -2621,17 +2546,11 @@
       <c r="D5" s="4" t="n">
         <v>1</v>
       </c>
-      <c r="F5" s="5" t="n">
-        <f aca="false">SUM(B5)/A5</f>
-        <v>0</v>
-      </c>
-      <c r="G5" s="5" t="n">
-        <f aca="false">SUM(C5)/A5</f>
-        <v>0</v>
-      </c>
+      <c r="F5" s="5"/>
+      <c r="G5" s="5"/>
       <c r="H5" s="5" t="n">
-        <f aca="false">SUM(D5)/A5</f>
-        <v>0.5</v>
+        <f aca="false">SUM(D4:D5)/A5</f>
+        <v>1</v>
       </c>
       <c r="J5" s="5" t="e">
         <f aca="false">SUMIF(B$4:B5,"=1")/SUMIF(B$4:B$23,"=1")</f>
@@ -2670,17 +2589,11 @@
       <c r="D6" s="4" t="n">
         <v>1</v>
       </c>
-      <c r="F6" s="5" t="n">
-        <f aca="false">SUM(B6)/A6</f>
-        <v>0</v>
-      </c>
-      <c r="G6" s="5" t="n">
-        <f aca="false">SUM(C6)/A6</f>
-        <v>0</v>
-      </c>
+      <c r="F6" s="5"/>
+      <c r="G6" s="5"/>
       <c r="H6" s="5" t="n">
-        <f aca="false">SUM(D6)/A6</f>
-        <v>0.333333333333333</v>
+        <f aca="false">SUM(D4:D6)/A6</f>
+        <v>1</v>
       </c>
       <c r="J6" s="5" t="e">
         <f aca="false">SUMIF(B$4:B6,"=1")/SUMIF(B$4:B$23,"=1")</f>
@@ -2719,17 +2632,11 @@
       <c r="D7" s="4" t="n">
         <v>0</v>
       </c>
-      <c r="F7" s="5" t="n">
-        <f aca="false">SUM(B7)/A7</f>
-        <v>0</v>
-      </c>
-      <c r="G7" s="5" t="n">
-        <f aca="false">SUM(C7)/A7</f>
-        <v>0</v>
-      </c>
+      <c r="F7" s="5"/>
+      <c r="G7" s="5"/>
       <c r="H7" s="5" t="n">
-        <f aca="false">SUM(D7)/A7</f>
-        <v>0</v>
+        <f aca="false">SUM(D4:D7)/A7</f>
+        <v>0.75</v>
       </c>
       <c r="J7" s="5" t="e">
         <f aca="false">SUMIF(B$4:B7,"=1")/SUMIF(B$4:B$23,"=1")</f>
@@ -2768,17 +2675,11 @@
       <c r="D8" s="4" t="n">
         <v>0</v>
       </c>
-      <c r="F8" s="5" t="n">
-        <f aca="false">SUM(B8)/A8</f>
-        <v>0</v>
-      </c>
-      <c r="G8" s="5" t="n">
-        <f aca="false">SUM(C8)/A8</f>
-        <v>0</v>
-      </c>
+      <c r="F8" s="5"/>
+      <c r="G8" s="5"/>
       <c r="H8" s="5" t="n">
-        <f aca="false">SUM(D8)/A8</f>
-        <v>0</v>
+        <f aca="false">SUM(D4:D8)/A8</f>
+        <v>0.6</v>
       </c>
       <c r="J8" s="5" t="e">
         <f aca="false">SUMIF(B$4:B8,"=1")/SUMIF(B$4:B$23,"=1")</f>
@@ -2805,7 +2706,7 @@
       </c>
       <c r="Q8" s="5" t="n">
         <f aca="false">_xlfn.MAXIFS(H$4:H$13,L$4:L$13,"&gt;="&amp;$N8)</f>
-        <v>0.5</v>
+        <v>1</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2815,18 +2716,9 @@
       <c r="B9" s="4"/>
       <c r="C9" s="4"/>
       <c r="D9" s="4"/>
-      <c r="F9" s="5" t="n">
-        <f aca="false">SUM(B9)/A9</f>
-        <v>0</v>
-      </c>
-      <c r="G9" s="5" t="n">
-        <f aca="false">SUM(C9)/A9</f>
-        <v>0</v>
-      </c>
-      <c r="H9" s="5" t="n">
-        <f aca="false">SUM(D9)/A9</f>
-        <v>0</v>
-      </c>
+      <c r="F9" s="5"/>
+      <c r="G9" s="5"/>
+      <c r="H9" s="5"/>
       <c r="J9" s="5" t="e">
         <f aca="false">SUMIF(B$4:B9,"=1")/SUMIF(B$4:B$23,"=1")</f>
         <v>#DIV/0!</v>
@@ -2852,7 +2744,7 @@
       </c>
       <c r="Q9" s="5" t="n">
         <f aca="false">_xlfn.MAXIFS(H$4:H$13,L$4:L$13,"&gt;="&amp;$N9)</f>
-        <v>0.5</v>
+        <v>1</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2862,18 +2754,9 @@
       <c r="B10" s="4"/>
       <c r="C10" s="4"/>
       <c r="D10" s="4"/>
-      <c r="F10" s="5" t="n">
-        <f aca="false">SUM(B10)/A10</f>
-        <v>0</v>
-      </c>
-      <c r="G10" s="5" t="n">
-        <f aca="false">SUM(C10)/A10</f>
-        <v>0</v>
-      </c>
-      <c r="H10" s="5" t="n">
-        <f aca="false">SUM(D10)/A10</f>
-        <v>0</v>
-      </c>
+      <c r="F10" s="5"/>
+      <c r="G10" s="5"/>
+      <c r="H10" s="5"/>
       <c r="J10" s="5" t="e">
         <f aca="false">SUMIF(B$4:B10,"=1")/SUMIF(B$4:B$23,"=1")</f>
         <v>#DIV/0!</v>
@@ -2899,7 +2782,7 @@
       </c>
       <c r="Q10" s="5" t="n">
         <f aca="false">_xlfn.MAXIFS(H$4:H$13,L$4:L$13,"&gt;="&amp;$N10)</f>
-        <v>0.5</v>
+        <v>1</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2909,18 +2792,9 @@
       <c r="B11" s="4"/>
       <c r="C11" s="4"/>
       <c r="D11" s="4"/>
-      <c r="F11" s="5" t="n">
-        <f aca="false">SUM(B11)/A11</f>
-        <v>0</v>
-      </c>
-      <c r="G11" s="5" t="n">
-        <f aca="false">SUM(C11)/A11</f>
-        <v>0</v>
-      </c>
-      <c r="H11" s="5" t="n">
-        <f aca="false">SUM(D11)/A11</f>
-        <v>0</v>
-      </c>
+      <c r="F11" s="5"/>
+      <c r="G11" s="5"/>
+      <c r="H11" s="5"/>
       <c r="J11" s="5" t="e">
         <f aca="false">SUMIF(B$4:B11,"=1")/SUMIF(B$4:B$23,"=1")</f>
         <v>#DIV/0!</v>
@@ -2946,7 +2820,7 @@
       </c>
       <c r="Q11" s="5" t="n">
         <f aca="false">_xlfn.MAXIFS(H$4:H$13,L$4:L$13,"&gt;="&amp;$N11)</f>
-        <v>0.333333333333333</v>
+        <v>1</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2956,18 +2830,9 @@
       <c r="B12" s="4"/>
       <c r="C12" s="4"/>
       <c r="D12" s="4"/>
-      <c r="F12" s="5" t="n">
-        <f aca="false">SUM(B12)/A12</f>
-        <v>0</v>
-      </c>
-      <c r="G12" s="5" t="n">
-        <f aca="false">SUM(C12)/A12</f>
-        <v>0</v>
-      </c>
-      <c r="H12" s="5" t="n">
-        <f aca="false">SUM(D12)/A12</f>
-        <v>0</v>
-      </c>
+      <c r="F12" s="5"/>
+      <c r="G12" s="5"/>
+      <c r="H12" s="5"/>
       <c r="J12" s="5" t="e">
         <f aca="false">SUMIF(B$4:B12,"=1")/SUMIF(B$4:B$23,"=1")</f>
         <v>#DIV/0!</v>
@@ -2993,7 +2858,7 @@
       </c>
       <c r="Q12" s="5" t="n">
         <f aca="false">_xlfn.MAXIFS(H$4:H$13,L$4:L$13,"&gt;="&amp;$N12)</f>
-        <v>0.333333333333333</v>
+        <v>1</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3003,18 +2868,9 @@
       <c r="B13" s="4"/>
       <c r="C13" s="4"/>
       <c r="D13" s="4"/>
-      <c r="F13" s="5" t="n">
-        <f aca="false">SUM(B13)/A13</f>
-        <v>0</v>
-      </c>
-      <c r="G13" s="5" t="n">
-        <f aca="false">SUM(C13)/A13</f>
-        <v>0</v>
-      </c>
-      <c r="H13" s="5" t="n">
-        <f aca="false">SUM(D13)/A13</f>
-        <v>0</v>
-      </c>
+      <c r="F13" s="5"/>
+      <c r="G13" s="5"/>
+      <c r="H13" s="5"/>
       <c r="J13" s="5" t="e">
         <f aca="false">SUMIF(B$4:B13,"=1")/SUMIF(B$4:B$23,"=1")</f>
         <v>#DIV/0!</v>
@@ -3040,7 +2896,7 @@
       </c>
       <c r="Q13" s="5" t="n">
         <f aca="false">_xlfn.MAXIFS(H$4:H$13,L$4:L$13,"&gt;="&amp;$N13)</f>
-        <v>0.333333333333333</v>
+        <v>1</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3067,7 +2923,7 @@
       </c>
       <c r="Q14" s="5" t="n">
         <f aca="false">_xlfn.MAXIFS(H$4:H$13,L$4:L$13,"&gt;="&amp;$N14)</f>
-        <v>0.333333333333333</v>
+        <v>1</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3182,17 +3038,17 @@
       <c r="E25" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="F25" s="5" t="n">
+      <c r="F25" s="5" t="e">
         <f aca="false">AVERAGE(F4:F13)</f>
-        <v>0</v>
+        <v>#DIV/0!</v>
       </c>
       <c r="G25" s="5" t="n">
         <f aca="false">AVERAGE(G4:G13)</f>
-        <v>0.1</v>
+        <v>1</v>
       </c>
       <c r="H25" s="5" t="n">
         <f aca="false">AVERAGE(H4:H13)</f>
-        <v>0.183333333333333</v>
+        <v>0.87</v>
       </c>
     </row>
   </sheetData>
@@ -3223,7 +3079,7 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.66015625" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="12.6796875" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="1" style="0" width="7.38"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="4.75"/>

</xml_diff>

<commit_message>
Fix metrics and add graphs
</commit_message>
<xml_diff>
--- a/solr/solrMetrics/q2/q2Metrics.xlsx
+++ b/solr/solrMetrics/q2/q2Metrics.xlsx
@@ -47,7 +47,7 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="11">
   <si>
-    <t xml:space="preserve">Q = Q2</t>
+    <t xml:space="preserve">Q = Q1</t>
   </si>
   <si>
     <t xml:space="preserve">Precision @</t>
@@ -128,6 +128,13 @@
       <charset val="1"/>
     </font>
     <font>
+      <sz val="8"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <family val="0"/>
+      <charset val="1"/>
+    </font>
+    <font>
       <sz val="18"/>
       <color rgb="FF757575"/>
       <name val="Arial"/>
@@ -136,11 +143,6 @@
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
-      <name val="Arial"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <sz val="9"/>
       <name val="Arial"/>
       <family val="2"/>
     </font>
@@ -193,7 +195,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="8">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -211,6 +213,10 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -294,7 +300,7 @@
 </styleSheet>
 </file>
 
-<file path=xl/charts/chart5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
@@ -322,7 +328,7 @@
                 <a:latin typeface="Arial"/>
                 <a:ea typeface="Arial"/>
               </a:rPr>
-              <a:t>Schemaless, Schema and Schema/M</a:t>
+              <a:t>PR-Curve Schemaless, Schema and Schema/M</a:t>
             </a:r>
           </a:p>
         </c:rich>
@@ -380,7 +386,6 @@
                 </a:pPr>
               </a:p>
             </c:txPr>
-            <c:dLblPos val="r"/>
             <c:showLegendKey val="0"/>
             <c:showVal val="0"/>
             <c:showCatName val="0"/>
@@ -396,48 +401,102 @@
           </c:dLbls>
           <c:cat>
             <c:strRef>
-              <c:f>'Query  eclipse  - Google, Bing,'!$A$4:$A$13</c:f>
+              <c:f>'Query  eclipse  - Google, Bing,'!$A$6:$A$23</c:f>
               <c:strCache>
-                <c:ptCount val="10"/>
+                <c:ptCount val="18"/>
                 <c:pt idx="0">
-                  <c:v>1</c:v>
+                  <c:v>3</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>2</c:v>
+                  <c:v>4</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>3</c:v>
+                  <c:v>5</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>4</c:v>
+                  <c:v>6</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>5</c:v>
+                  <c:v>7</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>6</c:v>
+                  <c:v>8</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>7</c:v>
+                  <c:v>9</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>8</c:v>
+                  <c:v>10</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>9</c:v>
+                  <c:v/>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>10</c:v>
+                  <c:v/>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v/>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v/>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v/>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v/>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v/>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v/>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v/>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v/>
                 </c:pt>
               </c:strCache>
             </c:strRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'Query  eclipse  - Google, Bing,'!$F$4:$F$13</c:f>
+              <c:f>'Query  eclipse  - Google, Bing,'!$F$4:$F$23</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="10"/>
+                <c:ptCount val="20"/>
+                <c:pt idx="0">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>0</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
@@ -483,7 +542,6 @@
                 </a:pPr>
               </a:p>
             </c:txPr>
-            <c:dLblPos val="r"/>
             <c:showLegendKey val="0"/>
             <c:showVal val="0"/>
             <c:showCatName val="0"/>
@@ -499,50 +557,101 @@
           </c:dLbls>
           <c:cat>
             <c:strRef>
-              <c:f>'Query  eclipse  - Google, Bing,'!$A$4:$A$13</c:f>
+              <c:f>'Query  eclipse  - Google, Bing,'!$A$6:$A$23</c:f>
               <c:strCache>
-                <c:ptCount val="10"/>
+                <c:ptCount val="18"/>
                 <c:pt idx="0">
-                  <c:v>1</c:v>
+                  <c:v>3</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>2</c:v>
+                  <c:v>4</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>3</c:v>
+                  <c:v>5</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>4</c:v>
+                  <c:v>6</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>5</c:v>
+                  <c:v>7</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>6</c:v>
+                  <c:v>8</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>7</c:v>
+                  <c:v>9</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>8</c:v>
+                  <c:v>10</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>9</c:v>
+                  <c:v/>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>10</c:v>
+                  <c:v/>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v/>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v/>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v/>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v/>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v/>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v/>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v/>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v/>
                 </c:pt>
               </c:strCache>
             </c:strRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'Query  eclipse  - Google, Bing,'!$G$4:$G$13</c:f>
+              <c:f>'Query  eclipse  - Google, Bing,'!$G$4:$G$23</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="10"/>
+                <c:ptCount val="20"/>
                 <c:pt idx="0">
                   <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.5</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.333333333333333</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.25</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.2</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.166666666666667</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.142857142857143</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0.125</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0.111111111111111</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>0.1</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -589,7 +698,6 @@
                 </a:pPr>
               </a:p>
             </c:txPr>
-            <c:dLblPos val="r"/>
             <c:showLegendKey val="0"/>
             <c:showVal val="0"/>
             <c:showCatName val="0"/>
@@ -605,48 +713,72 @@
           </c:dLbls>
           <c:cat>
             <c:strRef>
-              <c:f>'Query  eclipse  - Google, Bing,'!$A$4:$A$13</c:f>
+              <c:f>'Query  eclipse  - Google, Bing,'!$A$6:$A$23</c:f>
               <c:strCache>
-                <c:ptCount val="10"/>
+                <c:ptCount val="18"/>
                 <c:pt idx="0">
-                  <c:v>1</c:v>
+                  <c:v>3</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>2</c:v>
+                  <c:v>4</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>3</c:v>
+                  <c:v>5</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>4</c:v>
+                  <c:v>6</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>5</c:v>
+                  <c:v>7</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>6</c:v>
+                  <c:v>8</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>7</c:v>
+                  <c:v>9</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>8</c:v>
+                  <c:v>10</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>9</c:v>
+                  <c:v/>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>10</c:v>
+                  <c:v/>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v/>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v/>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v/>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v/>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v/>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v/>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v/>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v/>
                 </c:pt>
               </c:strCache>
             </c:strRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'Query  eclipse  - Google, Bing,'!$H$4:$H$13</c:f>
+              <c:f>'Query  eclipse  - Google, Bing,'!$H$4:$H$23</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="10"/>
+                <c:ptCount val="20"/>
                 <c:pt idx="0">
                   <c:v>1</c:v>
                 </c:pt>
@@ -661,6 +793,21 @@
                 </c:pt>
                 <c:pt idx="4">
                   <c:v>0.6</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.5</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.428571428571429</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0.375</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0.333333333333333</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>0.3</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -675,44 +822,16 @@
           </c:spPr>
         </c:hiLowLines>
         <c:marker val="0"/>
-        <c:axId val="6807767"/>
-        <c:axId val="65413307"/>
+        <c:axId val="24492165"/>
+        <c:axId val="44233378"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="6807767"/>
+        <c:axId val="24492165"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="b"/>
-        <c:title>
-          <c:tx>
-            <c:rich>
-              <a:bodyPr rot="0"/>
-              <a:lstStyle/>
-              <a:p>
-                <a:pPr>
-                  <a:defRPr b="0" sz="900" spc="-1" strike="noStrike">
-                    <a:latin typeface="Arial"/>
-                  </a:defRPr>
-                </a:pPr>
-                <a:r>
-                  <a:rPr b="0" sz="900" spc="-1" strike="noStrike">
-                    <a:latin typeface="Arial"/>
-                  </a:rPr>
-                  <a:t>Rank</a:t>
-                </a:r>
-              </a:p>
-            </c:rich>
-          </c:tx>
-          <c:overlay val="0"/>
-          <c:spPr>
-            <a:noFill/>
-            <a:ln w="0">
-              <a:noFill/>
-            </a:ln>
-          </c:spPr>
-        </c:title>
         <c:numFmt formatCode="General" sourceLinked="0"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
@@ -740,7 +859,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="65413307"/>
+        <c:crossAx val="44233378"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -748,7 +867,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="65413307"/>
+        <c:axId val="44233378"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -764,34 +883,6 @@
             </a:ln>
           </c:spPr>
         </c:majorGridlines>
-        <c:title>
-          <c:tx>
-            <c:rich>
-              <a:bodyPr rot="-5400000"/>
-              <a:lstStyle/>
-              <a:p>
-                <a:pPr>
-                  <a:defRPr b="0" sz="900" spc="-1" strike="noStrike">
-                    <a:latin typeface="Arial"/>
-                  </a:defRPr>
-                </a:pPr>
-                <a:r>
-                  <a:rPr b="0" sz="900" spc="-1" strike="noStrike">
-                    <a:latin typeface="Arial"/>
-                  </a:rPr>
-                  <a:t>Precision @</a:t>
-                </a:r>
-              </a:p>
-            </c:rich>
-          </c:tx>
-          <c:overlay val="0"/>
-          <c:spPr>
-            <a:noFill/>
-            <a:ln w="0">
-              <a:noFill/>
-            </a:ln>
-          </c:spPr>
-        </c:title>
         <c:numFmt formatCode="General" sourceLinked="0"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
@@ -819,7 +910,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="6807767"/>
+        <c:crossAx val="24492165"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -872,7 +963,7 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
@@ -900,7 +991,7 @@
                 <a:latin typeface="Arial"/>
                 <a:ea typeface="Arial"/>
               </a:rPr>
-              <a:t>Schemaless, Schema and Schema/M</a:t>
+              <a:t>Schemaless, Schema and Schema/M (Interpolated)</a:t>
             </a:r>
           </a:p>
         </c:rich>
@@ -958,7 +1049,6 @@
                 </a:pPr>
               </a:p>
             </c:txPr>
-            <c:dLblPos val="r"/>
             <c:showLegendKey val="0"/>
             <c:showVal val="0"/>
             <c:showCatName val="0"/>
@@ -1019,39 +1109,6 @@
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="11"/>
-                <c:pt idx="0">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>0</c:v>
-                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
@@ -1097,7 +1154,6 @@
                 </a:pPr>
               </a:p>
             </c:txPr>
-            <c:dLblPos val="r"/>
             <c:showLegendKey val="0"/>
             <c:showVal val="0"/>
             <c:showCatName val="0"/>
@@ -1158,39 +1214,6 @@
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="11"/>
-                <c:pt idx="0">
-                  <c:v>1</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>1</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>1</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>1</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>1</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>1</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>1</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>1</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>1</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>1</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>1</c:v>
-                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
@@ -1236,7 +1259,6 @@
                 </a:pPr>
               </a:p>
             </c:txPr>
-            <c:dLblPos val="r"/>
             <c:showLegendKey val="0"/>
             <c:showVal val="0"/>
             <c:showCatName val="0"/>
@@ -1297,39 +1319,6 @@
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="11"/>
-                <c:pt idx="0">
-                  <c:v>1</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>1</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>1</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>1</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>1</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>1</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>1</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>1</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>1</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>1</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>1</c:v>
-                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
@@ -1343,11 +1332,11 @@
           </c:spPr>
         </c:hiLowLines>
         <c:marker val="0"/>
-        <c:axId val="36929984"/>
-        <c:axId val="78329878"/>
+        <c:axId val="4443735"/>
+        <c:axId val="8918184"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="36929984"/>
+        <c:axId val="4443735"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1416,7 +1405,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="78329878"/>
+        <c:crossAx val="8918184"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1424,7 +1413,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="78329878"/>
+        <c:axId val="8918184"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1467,7 +1456,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="36929984"/>
+        <c:crossAx val="4443735"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1520,7 +1509,7 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart7.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart3.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
@@ -1595,7 +1584,6 @@
                 </a:pPr>
               </a:p>
             </c:txPr>
-            <c:dLblPos val="r"/>
             <c:showLegendKey val="0"/>
             <c:showVal val="0"/>
             <c:showCatName val="0"/>
@@ -1669,11 +1657,11 @@
           </c:spPr>
         </c:hiLowLines>
         <c:marker val="0"/>
-        <c:axId val="80334322"/>
-        <c:axId val="18610057"/>
+        <c:axId val="35912981"/>
+        <c:axId val="39965329"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="80334322"/>
+        <c:axId val="35912981"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1742,7 +1730,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="18610057"/>
+        <c:crossAx val="39965329"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1750,7 +1738,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="18610057"/>
+        <c:axId val="39965329"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1829,7 +1817,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="80334322"/>
+        <c:crossAx val="35912981"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1882,7 +1870,7 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart8.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart4.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
@@ -1968,7 +1956,6 @@
                 </a:pPr>
               </a:p>
             </c:txPr>
-            <c:dLblPos val="r"/>
             <c:showLegendKey val="0"/>
             <c:showVal val="0"/>
             <c:showCatName val="0"/>
@@ -2063,11 +2050,11 @@
           </c:spPr>
         </c:hiLowLines>
         <c:marker val="0"/>
-        <c:axId val="71905639"/>
-        <c:axId val="21640911"/>
+        <c:axId val="86251960"/>
+        <c:axId val="9500210"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="71905639"/>
+        <c:axId val="86251960"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2136,7 +2123,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="21640911"/>
+        <c:crossAx val="9500210"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -2144,7 +2131,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="21640911"/>
+        <c:axId val="9500210"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2223,7 +2210,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="71905639"/>
+        <c:crossAx val="86251960"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -2287,9 +2274,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>10</xdr:col>
-      <xdr:colOff>632520</xdr:colOff>
+      <xdr:colOff>633240</xdr:colOff>
       <xdr:row>42</xdr:row>
-      <xdr:rowOff>170640</xdr:rowOff>
+      <xdr:rowOff>171360</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
@@ -2297,8 +2284,8 @@
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
-        <a:off x="1440000" y="4924440"/>
-        <a:ext cx="5108040" cy="3151800"/>
+        <a:off x="1439280" y="5419800"/>
+        <a:ext cx="5105160" cy="3152520"/>
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
@@ -2317,9 +2304,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>18</xdr:col>
-      <xdr:colOff>427680</xdr:colOff>
+      <xdr:colOff>428400</xdr:colOff>
       <xdr:row>42</xdr:row>
-      <xdr:rowOff>103680</xdr:rowOff>
+      <xdr:rowOff>104400</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
@@ -2327,8 +2314,8 @@
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
-        <a:off x="7053480" y="4857480"/>
-        <a:ext cx="5116680" cy="3151800"/>
+        <a:off x="7048440" y="5352840"/>
+        <a:ext cx="5105160" cy="3152520"/>
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
@@ -2352,9 +2339,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>13</xdr:col>
-      <xdr:colOff>792720</xdr:colOff>
+      <xdr:colOff>793440</xdr:colOff>
       <xdr:row>26</xdr:row>
-      <xdr:rowOff>189360</xdr:rowOff>
+      <xdr:rowOff>190080</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
@@ -2362,8 +2349,8 @@
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
-        <a:off x="4648320" y="2724120"/>
-        <a:ext cx="4361760" cy="2665800"/>
+        <a:off x="4645800" y="2724120"/>
+        <a:ext cx="4352400" cy="2666520"/>
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
@@ -2382,9 +2369,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>8</xdr:col>
-      <xdr:colOff>801360</xdr:colOff>
+      <xdr:colOff>802080</xdr:colOff>
       <xdr:row>26</xdr:row>
-      <xdr:rowOff>189360</xdr:rowOff>
+      <xdr:rowOff>190080</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
@@ -2393,7 +2380,7 @@
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
         <a:off x="200160" y="2724120"/>
-        <a:ext cx="4351680" cy="2665800"/>
+        <a:ext cx="4352400" cy="2666520"/>
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
@@ -2414,10 +2401,10 @@
   <dimension ref="A1:Q25"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="L20" activeCellId="0" sqref="L20"/>
+      <selection pane="topLeft" activeCell="G13" activeCellId="0" sqref="G13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.6796875" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="12.640625" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="5.5"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="2" style="0" width="9.51"/>
@@ -2425,7 +2412,7 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="6" style="0" width="9.51"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="0" width="5.88"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="10" style="0" width="9.51"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="17" min="15" style="0" width="8.52"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="17" min="15" style="0" width="8.51"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2489,566 +2476,638 @@
         <v>6</v>
       </c>
     </row>
-    <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="4" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="4" t="n">
         <v>1</v>
       </c>
-      <c r="B4" s="4"/>
-      <c r="C4" s="4" t="n">
-        <v>1</v>
-      </c>
-      <c r="D4" s="4" t="n">
-        <v>1</v>
-      </c>
-      <c r="F4" s="5"/>
-      <c r="G4" s="5" t="n">
+      <c r="B4" s="5"/>
+      <c r="C4" s="5" t="n">
+        <v>1</v>
+      </c>
+      <c r="D4" s="5" t="n">
+        <v>1</v>
+      </c>
+      <c r="F4" s="6" t="n">
+        <f aca="false">SUM(B4)/A4</f>
+        <v>0</v>
+      </c>
+      <c r="G4" s="6" t="n">
         <f aca="false">SUM(C4)/A4</f>
         <v>1</v>
       </c>
-      <c r="H4" s="5" t="n">
+      <c r="H4" s="6" t="n">
         <f aca="false">SUM(D4)/A4</f>
         <v>1</v>
       </c>
-      <c r="J4" s="5" t="e">
+      <c r="J4" s="6" t="e">
         <f aca="false">SUMIF(B$4:B4,"=1")/SUMIF(B$4:B$23,"=1")</f>
         <v>#DIV/0!</v>
       </c>
-      <c r="K4" s="5" t="n">
+      <c r="K4" s="6" t="n">
         <f aca="false">SUMIF(C$4:C4,"=1")/SUMIF(C$4:C$23,"=1")</f>
         <v>1</v>
       </c>
-      <c r="L4" s="5" t="n">
+      <c r="L4" s="6" t="n">
         <f aca="false">SUMIF(D$4:D4,"=1")/SUMIF(D$4:D$23,"=1")</f>
         <v>0.333333333333333</v>
       </c>
-      <c r="N4" s="6" t="n">
+      <c r="N4" s="7" t="n">
         <v>0</v>
       </c>
-      <c r="O4" s="5" t="n">
-        <f aca="false">_xlfn.MAXIFS(F$4:F$13,J$4:J$13,"&gt;="&amp;$N4)</f>
-        <v>0</v>
-      </c>
-      <c r="P4" s="5" t="n">
-        <f aca="false">_xlfn.MAXIFS(G$4:G$13,K$4:K$13,"&gt;="&amp;$N4)</f>
-        <v>1</v>
-      </c>
-      <c r="Q4" s="5" t="n">
-        <f aca="false">_xlfn.MAXIFS(H$4:H$13,L$4:L$13,"&gt;="&amp;$N4)</f>
-        <v>1</v>
+      <c r="O4" s="6" t="e">
+        <f aca="false">maxifs(F$4:F$23,J$4:J$23,"&gt;="&amp;$N4)</f>
+        <v>#NAME?</v>
+      </c>
+      <c r="P4" s="6" t="e">
+        <f aca="false">maxifs(G$4:G$23,K$4:K$23,"&gt;="&amp;$N4)</f>
+        <v>#NAME?</v>
+      </c>
+      <c r="Q4" s="6" t="e">
+        <f aca="false">maxifs(H$4:H$23,L$4:L$23,"&gt;="&amp;$N4)</f>
+        <v>#NAME?</v>
       </c>
     </row>
-    <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="5" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="4" t="n">
         <v>2</v>
       </c>
-      <c r="B5" s="4"/>
-      <c r="C5" s="4"/>
-      <c r="D5" s="4" t="n">
-        <v>1</v>
-      </c>
-      <c r="F5" s="5"/>
-      <c r="G5" s="5"/>
-      <c r="H5" s="5" t="n">
-        <f aca="false">SUM(D4:D5)/A5</f>
-        <v>1</v>
-      </c>
-      <c r="J5" s="5" t="e">
+      <c r="B5" s="5"/>
+      <c r="C5" s="5"/>
+      <c r="D5" s="5" t="n">
+        <v>1</v>
+      </c>
+      <c r="F5" s="6" t="n">
+        <f aca="false">SUM(B$4:B5)/A5</f>
+        <v>0</v>
+      </c>
+      <c r="G5" s="6" t="n">
+        <f aca="false">SUM(C$4:C5)/A5</f>
+        <v>0.5</v>
+      </c>
+      <c r="H5" s="6" t="n">
+        <f aca="false">SUM(D$4:D5)/A5</f>
+        <v>1</v>
+      </c>
+      <c r="J5" s="6" t="e">
         <f aca="false">SUMIF(B$4:B5,"=1")/SUMIF(B$4:B$23,"=1")</f>
         <v>#DIV/0!</v>
       </c>
-      <c r="K5" s="5" t="n">
+      <c r="K5" s="6" t="n">
         <f aca="false">SUMIF(C$4:C5,"=1")/SUMIF(C$4:C$23,"=1")</f>
         <v>1</v>
       </c>
-      <c r="L5" s="5" t="n">
+      <c r="L5" s="6" t="n">
         <f aca="false">SUMIF(D$4:D5,"=1")/SUMIF(D$4:D$23,"=1")</f>
         <v>0.666666666666667</v>
       </c>
-      <c r="N5" s="6" t="n">
+      <c r="N5" s="7" t="n">
         <v>0.1</v>
       </c>
-      <c r="O5" s="5" t="n">
-        <f aca="false">_xlfn.MAXIFS(F$4:F$13,J$4:J$13,"&gt;="&amp;$N5)</f>
-        <v>0</v>
-      </c>
-      <c r="P5" s="5" t="n">
-        <f aca="false">_xlfn.MAXIFS(G$4:G$13,K$4:K$13,"&gt;="&amp;$N5)</f>
-        <v>1</v>
-      </c>
-      <c r="Q5" s="5" t="n">
-        <f aca="false">_xlfn.MAXIFS(H$4:H$13,L$4:L$13,"&gt;="&amp;$N5)</f>
-        <v>1</v>
+      <c r="O5" s="6" t="e">
+        <f aca="false">maxifs(F$4:F$23,J$4:J$23,"&gt;="&amp;$N5)</f>
+        <v>#NAME?</v>
+      </c>
+      <c r="P5" s="6" t="e">
+        <f aca="false">maxifs(G$4:G$23,K$4:K$23,"&gt;="&amp;$N5)</f>
+        <v>#NAME?</v>
+      </c>
+      <c r="Q5" s="6" t="e">
+        <f aca="false">maxifs(H$4:H$23,L$4:L$23,"&gt;="&amp;$N5)</f>
+        <v>#NAME?</v>
       </c>
     </row>
-    <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="6" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="4" t="n">
         <v>3</v>
       </c>
-      <c r="B6" s="4"/>
-      <c r="C6" s="4"/>
-      <c r="D6" s="4" t="n">
-        <v>1</v>
-      </c>
-      <c r="F6" s="5"/>
-      <c r="G6" s="5"/>
-      <c r="H6" s="5" t="n">
-        <f aca="false">SUM(D4:D6)/A6</f>
-        <v>1</v>
-      </c>
-      <c r="J6" s="5" t="e">
+      <c r="B6" s="5"/>
+      <c r="C6" s="5"/>
+      <c r="D6" s="5" t="n">
+        <v>1</v>
+      </c>
+      <c r="F6" s="6" t="n">
+        <f aca="false">SUM(B$4:B6)/A6</f>
+        <v>0</v>
+      </c>
+      <c r="G6" s="6" t="n">
+        <f aca="false">SUM(C$4:C6)/A6</f>
+        <v>0.333333333333333</v>
+      </c>
+      <c r="H6" s="6" t="n">
+        <f aca="false">SUM(D$4:D6)/A6</f>
+        <v>1</v>
+      </c>
+      <c r="J6" s="6" t="e">
         <f aca="false">SUMIF(B$4:B6,"=1")/SUMIF(B$4:B$23,"=1")</f>
         <v>#DIV/0!</v>
       </c>
-      <c r="K6" s="5" t="n">
+      <c r="K6" s="6" t="n">
         <f aca="false">SUMIF(C$4:C6,"=1")/SUMIF(C$4:C$23,"=1")</f>
         <v>1</v>
       </c>
-      <c r="L6" s="5" t="n">
+      <c r="L6" s="6" t="n">
         <f aca="false">SUMIF(D$4:D6,"=1")/SUMIF(D$4:D$23,"=1")</f>
         <v>1</v>
       </c>
-      <c r="N6" s="6" t="n">
+      <c r="N6" s="7" t="n">
         <v>0.2</v>
       </c>
-      <c r="O6" s="5" t="n">
-        <f aca="false">_xlfn.MAXIFS(F$4:F$13,J$4:J$13,"&gt;="&amp;$N6)</f>
-        <v>0</v>
-      </c>
-      <c r="P6" s="5" t="n">
-        <f aca="false">_xlfn.MAXIFS(G$4:G$13,K$4:K$13,"&gt;="&amp;$N6)</f>
-        <v>1</v>
-      </c>
-      <c r="Q6" s="5" t="n">
-        <f aca="false">_xlfn.MAXIFS(H$4:H$13,L$4:L$13,"&gt;="&amp;$N6)</f>
-        <v>1</v>
+      <c r="O6" s="6" t="e">
+        <f aca="false">maxifs(F$4:F$23,J$4:J$23,"&gt;="&amp;$N6)</f>
+        <v>#NAME?</v>
+      </c>
+      <c r="P6" s="6" t="e">
+        <f aca="false">maxifs(G$4:G$23,K$4:K$23,"&gt;="&amp;$N6)</f>
+        <v>#NAME?</v>
+      </c>
+      <c r="Q6" s="6" t="e">
+        <f aca="false">maxifs(H$4:H$23,L$4:L$23,"&gt;="&amp;$N6)</f>
+        <v>#NAME?</v>
       </c>
     </row>
-    <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="7" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="4" t="n">
         <v>4</v>
       </c>
-      <c r="B7" s="4"/>
-      <c r="C7" s="4"/>
-      <c r="D7" s="4" t="n">
+      <c r="B7" s="5"/>
+      <c r="C7" s="5"/>
+      <c r="D7" s="5" t="n">
         <v>0</v>
       </c>
-      <c r="F7" s="5"/>
-      <c r="G7" s="5"/>
-      <c r="H7" s="5" t="n">
-        <f aca="false">SUM(D4:D7)/A7</f>
+      <c r="F7" s="6" t="n">
+        <f aca="false">SUM(B$4:B7)/A7</f>
+        <v>0</v>
+      </c>
+      <c r="G7" s="6" t="n">
+        <f aca="false">SUM(C$4:C7)/A7</f>
+        <v>0.25</v>
+      </c>
+      <c r="H7" s="6" t="n">
+        <f aca="false">SUM(D$4:D7)/A7</f>
         <v>0.75</v>
       </c>
-      <c r="J7" s="5" t="e">
+      <c r="J7" s="6" t="e">
         <f aca="false">SUMIF(B$4:B7,"=1")/SUMIF(B$4:B$23,"=1")</f>
         <v>#DIV/0!</v>
       </c>
-      <c r="K7" s="5" t="n">
+      <c r="K7" s="6" t="n">
         <f aca="false">SUMIF(C$4:C7,"=1")/SUMIF(C$4:C$23,"=1")</f>
         <v>1</v>
       </c>
-      <c r="L7" s="5" t="n">
+      <c r="L7" s="6" t="n">
         <f aca="false">SUMIF(D$4:D7,"=1")/SUMIF(D$4:D$23,"=1")</f>
         <v>1</v>
       </c>
-      <c r="N7" s="6" t="n">
+      <c r="N7" s="7" t="n">
         <v>0.3</v>
       </c>
-      <c r="O7" s="5" t="n">
-        <f aca="false">_xlfn.MAXIFS(F$4:F$13,J$4:J$13,"&gt;="&amp;$N7)</f>
-        <v>0</v>
-      </c>
-      <c r="P7" s="5" t="n">
-        <f aca="false">_xlfn.MAXIFS(G$4:G$13,K$4:K$13,"&gt;="&amp;$N7)</f>
-        <v>1</v>
-      </c>
-      <c r="Q7" s="5" t="n">
-        <f aca="false">_xlfn.MAXIFS(H$4:H$13,L$4:L$13,"&gt;="&amp;$N7)</f>
-        <v>1</v>
+      <c r="O7" s="6" t="e">
+        <f aca="false">maxifs(F$4:F$23,J$4:J$23,"&gt;="&amp;$N7)</f>
+        <v>#NAME?</v>
+      </c>
+      <c r="P7" s="6" t="e">
+        <f aca="false">maxifs(G$4:G$23,K$4:K$23,"&gt;="&amp;$N7)</f>
+        <v>#NAME?</v>
+      </c>
+      <c r="Q7" s="6" t="e">
+        <f aca="false">maxifs(H$4:H$23,L$4:L$23,"&gt;="&amp;$N7)</f>
+        <v>#NAME?</v>
       </c>
     </row>
-    <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="8" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="4" t="n">
         <v>5</v>
       </c>
-      <c r="B8" s="4"/>
-      <c r="C8" s="4"/>
-      <c r="D8" s="4" t="n">
+      <c r="B8" s="5"/>
+      <c r="C8" s="5"/>
+      <c r="D8" s="5" t="n">
         <v>0</v>
       </c>
-      <c r="F8" s="5"/>
-      <c r="G8" s="5"/>
-      <c r="H8" s="5" t="n">
-        <f aca="false">SUM(D4:D8)/A8</f>
+      <c r="F8" s="6" t="n">
+        <f aca="false">SUM(B$4:B8)/A8</f>
+        <v>0</v>
+      </c>
+      <c r="G8" s="6" t="n">
+        <f aca="false">SUM(C$4:C8)/A8</f>
+        <v>0.2</v>
+      </c>
+      <c r="H8" s="6" t="n">
+        <f aca="false">SUM(D$4:D8)/A8</f>
         <v>0.6</v>
       </c>
-      <c r="J8" s="5" t="e">
+      <c r="J8" s="6" t="e">
         <f aca="false">SUMIF(B$4:B8,"=1")/SUMIF(B$4:B$23,"=1")</f>
         <v>#DIV/0!</v>
       </c>
-      <c r="K8" s="5" t="n">
+      <c r="K8" s="6" t="n">
         <f aca="false">SUMIF(C$4:C8,"=1")/SUMIF(C$4:C$23,"=1")</f>
         <v>1</v>
       </c>
-      <c r="L8" s="5" t="n">
+      <c r="L8" s="6" t="n">
         <f aca="false">SUMIF(D$4:D8,"=1")/SUMIF(D$4:D$23,"=1")</f>
         <v>1</v>
       </c>
-      <c r="N8" s="6" t="n">
+      <c r="N8" s="7" t="n">
         <v>0.4</v>
       </c>
-      <c r="O8" s="5" t="n">
-        <f aca="false">_xlfn.MAXIFS(F$4:F$13,J$4:J$13,"&gt;="&amp;$N8)</f>
-        <v>0</v>
-      </c>
-      <c r="P8" s="5" t="n">
-        <f aca="false">_xlfn.MAXIFS(G$4:G$13,K$4:K$13,"&gt;="&amp;$N8)</f>
-        <v>1</v>
-      </c>
-      <c r="Q8" s="5" t="n">
-        <f aca="false">_xlfn.MAXIFS(H$4:H$13,L$4:L$13,"&gt;="&amp;$N8)</f>
-        <v>1</v>
+      <c r="O8" s="6" t="e">
+        <f aca="false">maxifs(F$4:F$23,J$4:J$23,"&gt;="&amp;$N8)</f>
+        <v>#NAME?</v>
+      </c>
+      <c r="P8" s="6" t="e">
+        <f aca="false">maxifs(G$4:G$23,K$4:K$23,"&gt;="&amp;$N8)</f>
+        <v>#NAME?</v>
+      </c>
+      <c r="Q8" s="6" t="e">
+        <f aca="false">maxifs(H$4:H$23,L$4:L$23,"&gt;="&amp;$N8)</f>
+        <v>#NAME?</v>
       </c>
     </row>
-    <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="9" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="4" t="n">
         <v>6</v>
       </c>
-      <c r="B9" s="4"/>
-      <c r="C9" s="4"/>
-      <c r="D9" s="4"/>
-      <c r="F9" s="5"/>
-      <c r="G9" s="5"/>
-      <c r="H9" s="5"/>
-      <c r="J9" s="5" t="e">
+      <c r="B9" s="5"/>
+      <c r="C9" s="5"/>
+      <c r="D9" s="5"/>
+      <c r="F9" s="6" t="n">
+        <f aca="false">SUM(B$4:B9)/A9</f>
+        <v>0</v>
+      </c>
+      <c r="G9" s="6" t="n">
+        <f aca="false">SUM(C$4:C9)/A9</f>
+        <v>0.166666666666667</v>
+      </c>
+      <c r="H9" s="6" t="n">
+        <f aca="false">SUM(D$4:D9)/A9</f>
+        <v>0.5</v>
+      </c>
+      <c r="J9" s="6" t="e">
         <f aca="false">SUMIF(B$4:B9,"=1")/SUMIF(B$4:B$23,"=1")</f>
         <v>#DIV/0!</v>
       </c>
-      <c r="K9" s="5" t="n">
+      <c r="K9" s="6" t="n">
         <f aca="false">SUMIF(C$4:C9,"=1")/SUMIF(C$4:C$23,"=1")</f>
         <v>1</v>
       </c>
-      <c r="L9" s="5" t="n">
+      <c r="L9" s="6" t="n">
         <f aca="false">SUMIF(D$4:D9,"=1")/SUMIF(D$4:D$23,"=1")</f>
         <v>1</v>
       </c>
-      <c r="N9" s="6" t="n">
+      <c r="N9" s="7" t="n">
         <v>0.5</v>
       </c>
-      <c r="O9" s="5" t="n">
-        <f aca="false">_xlfn.MAXIFS(F$4:F$13,J$4:J$13,"&gt;="&amp;$N9)</f>
-        <v>0</v>
-      </c>
-      <c r="P9" s="5" t="n">
-        <f aca="false">_xlfn.MAXIFS(G$4:G$13,K$4:K$13,"&gt;="&amp;$N9)</f>
-        <v>1</v>
-      </c>
-      <c r="Q9" s="5" t="n">
-        <f aca="false">_xlfn.MAXIFS(H$4:H$13,L$4:L$13,"&gt;="&amp;$N9)</f>
-        <v>1</v>
+      <c r="O9" s="6" t="e">
+        <f aca="false">maxifs(F$4:F$23,J$4:J$23,"&gt;="&amp;$N9)</f>
+        <v>#NAME?</v>
+      </c>
+      <c r="P9" s="6" t="e">
+        <f aca="false">maxifs(G$4:G$23,K$4:K$23,"&gt;="&amp;$N9)</f>
+        <v>#NAME?</v>
+      </c>
+      <c r="Q9" s="6" t="e">
+        <f aca="false">maxifs(H$4:H$23,L$4:L$23,"&gt;="&amp;$N9)</f>
+        <v>#NAME?</v>
       </c>
     </row>
-    <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="10" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="4" t="n">
         <v>7</v>
       </c>
-      <c r="B10" s="4"/>
-      <c r="C10" s="4"/>
-      <c r="D10" s="4"/>
-      <c r="F10" s="5"/>
-      <c r="G10" s="5"/>
-      <c r="H10" s="5"/>
-      <c r="J10" s="5" t="e">
+      <c r="B10" s="5"/>
+      <c r="C10" s="5"/>
+      <c r="D10" s="5"/>
+      <c r="F10" s="6" t="n">
+        <f aca="false">SUM(B$4:B10)/A10</f>
+        <v>0</v>
+      </c>
+      <c r="G10" s="6" t="n">
+        <f aca="false">SUM(C$4:C10)/A10</f>
+        <v>0.142857142857143</v>
+      </c>
+      <c r="H10" s="6" t="n">
+        <f aca="false">SUM(D$4:D10)/A10</f>
+        <v>0.428571428571429</v>
+      </c>
+      <c r="J10" s="6" t="e">
         <f aca="false">SUMIF(B$4:B10,"=1")/SUMIF(B$4:B$23,"=1")</f>
         <v>#DIV/0!</v>
       </c>
-      <c r="K10" s="5" t="n">
+      <c r="K10" s="6" t="n">
         <f aca="false">SUMIF(C$4:C10,"=1")/SUMIF(C$4:C$23,"=1")</f>
         <v>1</v>
       </c>
-      <c r="L10" s="5" t="n">
+      <c r="L10" s="6" t="n">
         <f aca="false">SUMIF(D$4:D10,"=1")/SUMIF(D$4:D$23,"=1")</f>
         <v>1</v>
       </c>
-      <c r="N10" s="6" t="n">
+      <c r="N10" s="7" t="n">
         <v>0.6</v>
       </c>
-      <c r="O10" s="5" t="n">
-        <f aca="false">_xlfn.MAXIFS(F$4:F$13,J$4:J$13,"&gt;="&amp;$N10)</f>
-        <v>0</v>
-      </c>
-      <c r="P10" s="5" t="n">
-        <f aca="false">_xlfn.MAXIFS(G$4:G$13,K$4:K$13,"&gt;="&amp;$N10)</f>
-        <v>1</v>
-      </c>
-      <c r="Q10" s="5" t="n">
-        <f aca="false">_xlfn.MAXIFS(H$4:H$13,L$4:L$13,"&gt;="&amp;$N10)</f>
-        <v>1</v>
+      <c r="O10" s="6" t="e">
+        <f aca="false">maxifs(F$4:F$23,J$4:J$23,"&gt;="&amp;$N10)</f>
+        <v>#NAME?</v>
+      </c>
+      <c r="P10" s="6" t="e">
+        <f aca="false">maxifs(G$4:G$23,K$4:K$23,"&gt;="&amp;$N10)</f>
+        <v>#NAME?</v>
+      </c>
+      <c r="Q10" s="6" t="e">
+        <f aca="false">maxifs(H$4:H$23,L$4:L$23,"&gt;="&amp;$N10)</f>
+        <v>#NAME?</v>
       </c>
     </row>
-    <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="11" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="4" t="n">
         <v>8</v>
       </c>
-      <c r="B11" s="4"/>
-      <c r="C11" s="4"/>
-      <c r="D11" s="4"/>
-      <c r="F11" s="5"/>
-      <c r="G11" s="5"/>
-      <c r="H11" s="5"/>
-      <c r="J11" s="5" t="e">
+      <c r="B11" s="5"/>
+      <c r="C11" s="5"/>
+      <c r="D11" s="5"/>
+      <c r="F11" s="6" t="n">
+        <f aca="false">SUM(B$4:B11)/A11</f>
+        <v>0</v>
+      </c>
+      <c r="G11" s="6" t="n">
+        <f aca="false">SUM(C$4:C11)/A11</f>
+        <v>0.125</v>
+      </c>
+      <c r="H11" s="6" t="n">
+        <f aca="false">SUM(D$4:D11)/A11</f>
+        <v>0.375</v>
+      </c>
+      <c r="J11" s="6" t="e">
         <f aca="false">SUMIF(B$4:B11,"=1")/SUMIF(B$4:B$23,"=1")</f>
         <v>#DIV/0!</v>
       </c>
-      <c r="K11" s="5" t="n">
+      <c r="K11" s="6" t="n">
         <f aca="false">SUMIF(C$4:C11,"=1")/SUMIF(C$4:C$23,"=1")</f>
         <v>1</v>
       </c>
-      <c r="L11" s="5" t="n">
+      <c r="L11" s="6" t="n">
         <f aca="false">SUMIF(D$4:D11,"=1")/SUMIF(D$4:D$23,"=1")</f>
         <v>1</v>
       </c>
-      <c r="N11" s="6" t="n">
+      <c r="N11" s="7" t="n">
         <v>0.7</v>
       </c>
-      <c r="O11" s="5" t="n">
-        <f aca="false">_xlfn.MAXIFS(F$4:F$13,J$4:J$13,"&gt;="&amp;$N11)</f>
-        <v>0</v>
-      </c>
-      <c r="P11" s="5" t="n">
-        <f aca="false">_xlfn.MAXIFS(G$4:G$13,K$4:K$13,"&gt;="&amp;$N11)</f>
-        <v>1</v>
-      </c>
-      <c r="Q11" s="5" t="n">
-        <f aca="false">_xlfn.MAXIFS(H$4:H$13,L$4:L$13,"&gt;="&amp;$N11)</f>
-        <v>1</v>
+      <c r="O11" s="6" t="e">
+        <f aca="false">maxifs(F$4:F$23,J$4:J$23,"&gt;="&amp;$N11)</f>
+        <v>#NAME?</v>
+      </c>
+      <c r="P11" s="6" t="e">
+        <f aca="false">maxifs(G$4:G$23,K$4:K$23,"&gt;="&amp;$N11)</f>
+        <v>#NAME?</v>
+      </c>
+      <c r="Q11" s="6" t="e">
+        <f aca="false">maxifs(H$4:H$23,L$4:L$23,"&gt;="&amp;$N11)</f>
+        <v>#NAME?</v>
       </c>
     </row>
-    <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="12" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="4" t="n">
         <v>9</v>
       </c>
-      <c r="B12" s="4"/>
-      <c r="C12" s="4"/>
-      <c r="D12" s="4"/>
-      <c r="F12" s="5"/>
-      <c r="G12" s="5"/>
-      <c r="H12" s="5"/>
-      <c r="J12" s="5" t="e">
+      <c r="B12" s="5"/>
+      <c r="C12" s="5"/>
+      <c r="D12" s="5"/>
+      <c r="F12" s="6" t="n">
+        <f aca="false">SUM(B$4:B12)/A12</f>
+        <v>0</v>
+      </c>
+      <c r="G12" s="6" t="n">
+        <f aca="false">SUM(C$4:C12)/A12</f>
+        <v>0.111111111111111</v>
+      </c>
+      <c r="H12" s="6" t="n">
+        <f aca="false">SUM(D$4:D12)/A12</f>
+        <v>0.333333333333333</v>
+      </c>
+      <c r="J12" s="6" t="e">
         <f aca="false">SUMIF(B$4:B12,"=1")/SUMIF(B$4:B$23,"=1")</f>
         <v>#DIV/0!</v>
       </c>
-      <c r="K12" s="5" t="n">
+      <c r="K12" s="6" t="n">
         <f aca="false">SUMIF(C$4:C12,"=1")/SUMIF(C$4:C$23,"=1")</f>
         <v>1</v>
       </c>
-      <c r="L12" s="5" t="n">
+      <c r="L12" s="6" t="n">
         <f aca="false">SUMIF(D$4:D12,"=1")/SUMIF(D$4:D$23,"=1")</f>
         <v>1</v>
       </c>
-      <c r="N12" s="6" t="n">
+      <c r="N12" s="7" t="n">
         <v>0.8</v>
       </c>
-      <c r="O12" s="5" t="n">
-        <f aca="false">_xlfn.MAXIFS(F$4:F$13,J$4:J$13,"&gt;="&amp;$N12)</f>
-        <v>0</v>
-      </c>
-      <c r="P12" s="5" t="n">
-        <f aca="false">_xlfn.MAXIFS(G$4:G$13,K$4:K$13,"&gt;="&amp;$N12)</f>
-        <v>1</v>
-      </c>
-      <c r="Q12" s="5" t="n">
-        <f aca="false">_xlfn.MAXIFS(H$4:H$13,L$4:L$13,"&gt;="&amp;$N12)</f>
-        <v>1</v>
+      <c r="O12" s="6" t="e">
+        <f aca="false">maxifs(F$4:F$23,J$4:J$23,"&gt;="&amp;$N12)</f>
+        <v>#NAME?</v>
+      </c>
+      <c r="P12" s="6" t="e">
+        <f aca="false">maxifs(G$4:G$23,K$4:K$23,"&gt;="&amp;$N12)</f>
+        <v>#NAME?</v>
+      </c>
+      <c r="Q12" s="6" t="e">
+        <f aca="false">maxifs(H$4:H$23,L$4:L$23,"&gt;="&amp;$N12)</f>
+        <v>#NAME?</v>
       </c>
     </row>
-    <row r="13" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="13" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="4" t="n">
         <v>10</v>
       </c>
-      <c r="B13" s="4"/>
-      <c r="C13" s="4"/>
-      <c r="D13" s="4"/>
-      <c r="F13" s="5"/>
-      <c r="G13" s="5"/>
-      <c r="H13" s="5"/>
-      <c r="J13" s="5" t="e">
+      <c r="B13" s="5"/>
+      <c r="C13" s="5"/>
+      <c r="D13" s="5"/>
+      <c r="F13" s="6" t="n">
+        <f aca="false">SUM(B$4:B13)/A13</f>
+        <v>0</v>
+      </c>
+      <c r="G13" s="6" t="n">
+        <f aca="false">SUM(C$4:C13)/A13</f>
+        <v>0.1</v>
+      </c>
+      <c r="H13" s="6" t="n">
+        <f aca="false">SUM(D$4:D13)/A13</f>
+        <v>0.3</v>
+      </c>
+      <c r="J13" s="6" t="e">
         <f aca="false">SUMIF(B$4:B13,"=1")/SUMIF(B$4:B$23,"=1")</f>
         <v>#DIV/0!</v>
       </c>
-      <c r="K13" s="5" t="n">
+      <c r="K13" s="6" t="n">
         <f aca="false">SUMIF(C$4:C13,"=1")/SUMIF(C$4:C$23,"=1")</f>
         <v>1</v>
       </c>
-      <c r="L13" s="5" t="n">
+      <c r="L13" s="6" t="n">
         <f aca="false">SUMIF(D$4:D13,"=1")/SUMIF(D$4:D$23,"=1")</f>
         <v>1</v>
       </c>
-      <c r="N13" s="6" t="n">
+      <c r="N13" s="7" t="n">
         <v>0.9</v>
       </c>
-      <c r="O13" s="5" t="n">
-        <f aca="false">_xlfn.MAXIFS(F$4:F$13,J$4:J$13,"&gt;="&amp;$N13)</f>
-        <v>0</v>
-      </c>
-      <c r="P13" s="5" t="n">
-        <f aca="false">_xlfn.MAXIFS(G$4:G$13,K$4:K$13,"&gt;="&amp;$N13)</f>
-        <v>1</v>
-      </c>
-      <c r="Q13" s="5" t="n">
-        <f aca="false">_xlfn.MAXIFS(H$4:H$13,L$4:L$13,"&gt;="&amp;$N13)</f>
-        <v>1</v>
+      <c r="O13" s="6" t="e">
+        <f aca="false">maxifs(F$4:F$23,J$4:J$23,"&gt;="&amp;$N13)</f>
+        <v>#NAME?</v>
+      </c>
+      <c r="P13" s="6" t="e">
+        <f aca="false">maxifs(G$4:G$23,K$4:K$23,"&gt;="&amp;$N13)</f>
+        <v>#NAME?</v>
+      </c>
+      <c r="Q13" s="6" t="e">
+        <f aca="false">maxifs(H$4:H$23,L$4:L$23,"&gt;="&amp;$N13)</f>
+        <v>#NAME?</v>
       </c>
     </row>
-    <row r="14" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="14" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="4"/>
       <c r="B14" s="4"/>
       <c r="C14" s="4"/>
       <c r="D14" s="4"/>
-      <c r="F14" s="5"/>
-      <c r="G14" s="5"/>
-      <c r="H14" s="5"/>
-      <c r="J14" s="5"/>
-      <c r="K14" s="5"/>
-      <c r="L14" s="5"/>
-      <c r="N14" s="6" t="n">
-        <v>1</v>
-      </c>
-      <c r="O14" s="5" t="n">
-        <f aca="false">_xlfn.MAXIFS(F$4:F$13,J$4:J$13,"&gt;="&amp;$N14)</f>
-        <v>0</v>
-      </c>
-      <c r="P14" s="5" t="n">
-        <f aca="false">_xlfn.MAXIFS(G$4:G$13,K$4:K$13,"&gt;="&amp;$N14)</f>
-        <v>1</v>
-      </c>
-      <c r="Q14" s="5" t="n">
-        <f aca="false">_xlfn.MAXIFS(H$4:H$13,L$4:L$13,"&gt;="&amp;$N14)</f>
-        <v>1</v>
+      <c r="F14" s="6"/>
+      <c r="G14" s="6"/>
+      <c r="H14" s="6"/>
+      <c r="J14" s="6"/>
+      <c r="K14" s="6"/>
+      <c r="L14" s="6"/>
+      <c r="N14" s="7" t="n">
+        <v>1</v>
+      </c>
+      <c r="O14" s="6" t="e">
+        <f aca="false">maxifs(F$4:F$23,J$4:J$23,"&gt;="&amp;$N14)</f>
+        <v>#NAME?</v>
+      </c>
+      <c r="P14" s="6" t="e">
+        <f aca="false">maxifs(G$4:G$23,K$4:K$23,"&gt;="&amp;$N14)</f>
+        <v>#NAME?</v>
+      </c>
+      <c r="Q14" s="6" t="e">
+        <f aca="false">maxifs(H$4:H$23,L$4:L$23,"&gt;="&amp;$N14)</f>
+        <v>#NAME?</v>
       </c>
     </row>
-    <row r="15" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="15" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="4"/>
       <c r="B15" s="4"/>
       <c r="C15" s="4"/>
       <c r="D15" s="4"/>
-      <c r="F15" s="5"/>
-      <c r="G15" s="5"/>
-      <c r="H15" s="5"/>
-      <c r="J15" s="5"/>
-      <c r="K15" s="5"/>
-      <c r="L15" s="5"/>
+      <c r="F15" s="6"/>
+      <c r="G15" s="6"/>
+      <c r="H15" s="6"/>
+      <c r="J15" s="6"/>
+      <c r="K15" s="6"/>
+      <c r="L15" s="6"/>
     </row>
-    <row r="16" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="16" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="4"/>
       <c r="B16" s="4"/>
       <c r="C16" s="4"/>
       <c r="D16" s="4"/>
-      <c r="F16" s="5"/>
-      <c r="G16" s="5"/>
-      <c r="H16" s="5"/>
-      <c r="J16" s="5"/>
-      <c r="K16" s="5"/>
-      <c r="L16" s="5"/>
+      <c r="F16" s="6"/>
+      <c r="G16" s="6"/>
+      <c r="H16" s="6"/>
+      <c r="J16" s="6"/>
+      <c r="K16" s="6"/>
+      <c r="L16" s="6"/>
     </row>
-    <row r="17" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="17" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="4"/>
       <c r="B17" s="4"/>
       <c r="C17" s="4"/>
       <c r="D17" s="4"/>
-      <c r="F17" s="5"/>
-      <c r="G17" s="5"/>
-      <c r="H17" s="5"/>
-      <c r="J17" s="5"/>
-      <c r="K17" s="5"/>
-      <c r="L17" s="5"/>
+      <c r="F17" s="6"/>
+      <c r="G17" s="6"/>
+      <c r="H17" s="6"/>
+      <c r="J17" s="6"/>
+      <c r="K17" s="6"/>
+      <c r="L17" s="6"/>
     </row>
-    <row r="18" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="18" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="4"/>
       <c r="B18" s="4"/>
       <c r="C18" s="4"/>
       <c r="D18" s="4"/>
-      <c r="F18" s="5"/>
-      <c r="G18" s="5"/>
-      <c r="H18" s="5"/>
-      <c r="J18" s="5"/>
-      <c r="K18" s="5"/>
-      <c r="L18" s="5"/>
+      <c r="F18" s="6"/>
+      <c r="G18" s="6"/>
+      <c r="H18" s="6"/>
+      <c r="J18" s="6"/>
+      <c r="K18" s="6"/>
+      <c r="L18" s="6"/>
     </row>
-    <row r="19" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="19" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="4"/>
       <c r="B19" s="4"/>
       <c r="C19" s="4"/>
       <c r="D19" s="4"/>
-      <c r="F19" s="5"/>
-      <c r="G19" s="5"/>
-      <c r="H19" s="5"/>
-      <c r="J19" s="5"/>
-      <c r="K19" s="5"/>
-      <c r="L19" s="5"/>
+      <c r="F19" s="6"/>
+      <c r="G19" s="6"/>
+      <c r="H19" s="6"/>
+      <c r="J19" s="6"/>
+      <c r="K19" s="6"/>
+      <c r="L19" s="6"/>
     </row>
-    <row r="20" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="20" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="4"/>
       <c r="B20" s="4"/>
       <c r="C20" s="4"/>
       <c r="D20" s="4"/>
-      <c r="F20" s="5"/>
-      <c r="G20" s="5"/>
-      <c r="H20" s="5"/>
-      <c r="J20" s="5"/>
-      <c r="K20" s="5"/>
-      <c r="L20" s="5"/>
+      <c r="F20" s="6"/>
+      <c r="G20" s="6"/>
+      <c r="H20" s="6"/>
+      <c r="J20" s="6"/>
+      <c r="K20" s="6"/>
+      <c r="L20" s="6"/>
     </row>
-    <row r="21" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="21" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="4"/>
       <c r="B21" s="4"/>
       <c r="C21" s="4"/>
       <c r="D21" s="4"/>
-      <c r="F21" s="5"/>
-      <c r="G21" s="5"/>
-      <c r="H21" s="5"/>
-      <c r="J21" s="5"/>
-      <c r="K21" s="5"/>
-      <c r="L21" s="5"/>
+      <c r="F21" s="6"/>
+      <c r="G21" s="6"/>
+      <c r="H21" s="6"/>
+      <c r="J21" s="6"/>
+      <c r="K21" s="6"/>
+      <c r="L21" s="6"/>
     </row>
-    <row r="22" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="22" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="4"/>
       <c r="B22" s="4"/>
       <c r="C22" s="4"/>
       <c r="D22" s="4"/>
-      <c r="F22" s="5"/>
-      <c r="G22" s="5"/>
-      <c r="H22" s="5"/>
-      <c r="J22" s="5"/>
-      <c r="K22" s="5"/>
-      <c r="L22" s="5"/>
+      <c r="F22" s="6"/>
+      <c r="G22" s="6"/>
+      <c r="H22" s="6"/>
+      <c r="J22" s="6"/>
+      <c r="K22" s="6"/>
+      <c r="L22" s="6"/>
     </row>
-    <row r="23" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="23" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="4"/>
       <c r="B23" s="4"/>
       <c r="C23" s="4"/>
       <c r="D23" s="4"/>
-      <c r="F23" s="5"/>
-      <c r="G23" s="5"/>
-      <c r="H23" s="5"/>
-      <c r="J23" s="5"/>
-      <c r="K23" s="5"/>
-      <c r="L23" s="5"/>
+      <c r="F23" s="6"/>
+      <c r="G23" s="6"/>
+      <c r="H23" s="6"/>
+      <c r="J23" s="6"/>
+      <c r="K23" s="6"/>
+      <c r="L23" s="6"/>
     </row>
     <row r="25" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="E25" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="F25" s="5" t="e">
-        <f aca="false">AVERAGE(F4:F13)</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="G25" s="5" t="n">
-        <f aca="false">AVERAGE(G4:G13)</f>
-        <v>1</v>
-      </c>
-      <c r="H25" s="5" t="n">
-        <f aca="false">AVERAGE(H4:H13)</f>
-        <v>0.87</v>
+      <c r="F25" s="6" t="n">
+        <f aca="false">AVERAGE(F4:F23)</f>
+        <v>0</v>
+      </c>
+      <c r="G25" s="6" t="n">
+        <f aca="false">AVERAGE(G4:G23)</f>
+        <v>0.292896825396825</v>
+      </c>
+      <c r="H25" s="6" t="n">
+        <f aca="false">AVERAGE(H4:H23)</f>
+        <v>0.628690476190476</v>
       </c>
     </row>
   </sheetData>
@@ -3079,7 +3138,7 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.6796875" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="12.640625" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="1" style="0" width="7.38"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="4.75"/>
@@ -3104,10 +3163,10 @@
         <v>7</v>
       </c>
       <c r="F3" s="4"/>
-      <c r="G3" s="6" t="n">
+      <c r="G3" s="7" t="n">
         <v>0</v>
       </c>
-      <c r="H3" s="5" t="e">
+      <c r="H3" s="6" t="e">
         <f aca="false">maxifs(D$4:D$13,E$4:E$13,"&gt;="&amp;G3)</f>
         <v>#NAME?</v>
       </c>
@@ -3120,19 +3179,19 @@
         <v>1</v>
       </c>
       <c r="C4" s="4"/>
-      <c r="D4" s="5" t="n">
+      <c r="D4" s="6" t="n">
         <f aca="false">COUNTIF(B$4:B4, "=1")/COUNTA(B$4:B4)</f>
         <v>1</v>
       </c>
-      <c r="E4" s="6" t="n">
+      <c r="E4" s="7" t="n">
         <f aca="false">COUNTIF(B$4:B4, "=1")/COUNTIF(B$4:B$13,"=1")</f>
         <v>0.2</v>
       </c>
       <c r="F4" s="4"/>
-      <c r="G4" s="6" t="n">
+      <c r="G4" s="7" t="n">
         <v>0.1</v>
       </c>
-      <c r="H4" s="5" t="e">
+      <c r="H4" s="6" t="e">
         <f aca="false">maxifs(D$4:D$13,E$4:E$13,"&gt;="&amp;G4)</f>
         <v>#NAME?</v>
       </c>
@@ -3145,19 +3204,19 @@
         <v>1</v>
       </c>
       <c r="C5" s="4"/>
-      <c r="D5" s="5" t="n">
+      <c r="D5" s="6" t="n">
         <f aca="false">COUNTIF(B$4:B5, "=1")/COUNTA(B$4:B5)</f>
         <v>1</v>
       </c>
-      <c r="E5" s="6" t="n">
+      <c r="E5" s="7" t="n">
         <f aca="false">COUNTIF(B$4:B5, "=1")/COUNTIF(B$4:B$13,"=1")</f>
         <v>0.4</v>
       </c>
       <c r="F5" s="4"/>
-      <c r="G5" s="6" t="n">
+      <c r="G5" s="7" t="n">
         <v>0.2</v>
       </c>
-      <c r="H5" s="5" t="e">
+      <c r="H5" s="6" t="e">
         <f aca="false">maxifs(D$4:D$13,E$4:E$13,"&gt;="&amp;G5)</f>
         <v>#NAME?</v>
       </c>
@@ -3170,19 +3229,19 @@
         <v>0</v>
       </c>
       <c r="C6" s="4"/>
-      <c r="D6" s="5" t="n">
+      <c r="D6" s="6" t="n">
         <f aca="false">COUNTIF(B$4:B6, "=1")/COUNTA(B$4:B6)</f>
         <v>0.666666666666667</v>
       </c>
-      <c r="E6" s="6" t="n">
+      <c r="E6" s="7" t="n">
         <f aca="false">COUNTIF(B$4:B6, "=1")/COUNTIF(B$4:B$13,"=1")</f>
         <v>0.4</v>
       </c>
       <c r="F6" s="4"/>
-      <c r="G6" s="6" t="n">
+      <c r="G6" s="7" t="n">
         <v>0.3</v>
       </c>
-      <c r="H6" s="5" t="e">
+      <c r="H6" s="6" t="e">
         <f aca="false">maxifs(D$4:D$13,E$4:E$13,"&gt;="&amp;G6)</f>
         <v>#NAME?</v>
       </c>
@@ -3195,19 +3254,19 @@
         <v>1</v>
       </c>
       <c r="C7" s="4"/>
-      <c r="D7" s="5" t="n">
+      <c r="D7" s="6" t="n">
         <f aca="false">COUNTIF(B$4:B7, "=1")/COUNTA(B$4:B7)</f>
         <v>0.75</v>
       </c>
-      <c r="E7" s="6" t="n">
+      <c r="E7" s="7" t="n">
         <f aca="false">COUNTIF(B$4:B7, "=1")/COUNTIF(B$4:B$13,"=1")</f>
         <v>0.6</v>
       </c>
       <c r="F7" s="4"/>
-      <c r="G7" s="6" t="n">
+      <c r="G7" s="7" t="n">
         <v>0.4</v>
       </c>
-      <c r="H7" s="5" t="e">
+      <c r="H7" s="6" t="e">
         <f aca="false">maxifs(D$4:D$13,E$4:E$13,"&gt;="&amp;G7)</f>
         <v>#NAME?</v>
       </c>
@@ -3220,19 +3279,19 @@
         <v>0</v>
       </c>
       <c r="C8" s="4"/>
-      <c r="D8" s="5" t="n">
+      <c r="D8" s="6" t="n">
         <f aca="false">COUNTIF(B$4:B8, "=1")/COUNTA(B$4:B8)</f>
         <v>0.6</v>
       </c>
-      <c r="E8" s="6" t="n">
+      <c r="E8" s="7" t="n">
         <f aca="false">COUNTIF(B$4:B8, "=1")/COUNTIF(B$4:B$13,"=1")</f>
         <v>0.6</v>
       </c>
       <c r="F8" s="4"/>
-      <c r="G8" s="6" t="n">
+      <c r="G8" s="7" t="n">
         <v>0.5</v>
       </c>
-      <c r="H8" s="5" t="e">
+      <c r="H8" s="6" t="e">
         <f aca="false">maxifs(D$4:D$13,E$4:E$13,"&gt;="&amp;G8)</f>
         <v>#NAME?</v>
       </c>
@@ -3245,19 +3304,19 @@
         <v>0</v>
       </c>
       <c r="C9" s="4"/>
-      <c r="D9" s="5" t="n">
+      <c r="D9" s="6" t="n">
         <f aca="false">COUNTIF(B$4:B9, "=1")/COUNTA(B$4:B9)</f>
         <v>0.5</v>
       </c>
-      <c r="E9" s="6" t="n">
+      <c r="E9" s="7" t="n">
         <f aca="false">COUNTIF(B$4:B9, "=1")/COUNTIF(B$4:B$13,"=1")</f>
         <v>0.6</v>
       </c>
       <c r="F9" s="4"/>
-      <c r="G9" s="6" t="n">
+      <c r="G9" s="7" t="n">
         <v>0.6</v>
       </c>
-      <c r="H9" s="5" t="e">
+      <c r="H9" s="6" t="e">
         <f aca="false">maxifs(D$4:D$13,E$4:E$13,"&gt;="&amp;G9)</f>
         <v>#NAME?</v>
       </c>
@@ -3270,19 +3329,19 @@
         <v>1</v>
       </c>
       <c r="C10" s="4"/>
-      <c r="D10" s="5" t="n">
+      <c r="D10" s="6" t="n">
         <f aca="false">COUNTIF(B$4:B10, "=1")/COUNTA(B$4:B10)</f>
         <v>0.571428571428571</v>
       </c>
-      <c r="E10" s="6" t="n">
+      <c r="E10" s="7" t="n">
         <f aca="false">COUNTIF(B$4:B10, "=1")/COUNTIF(B$4:B$13,"=1")</f>
         <v>0.8</v>
       </c>
       <c r="F10" s="4"/>
-      <c r="G10" s="6" t="n">
+      <c r="G10" s="7" t="n">
         <v>0.7</v>
       </c>
-      <c r="H10" s="5" t="e">
+      <c r="H10" s="6" t="e">
         <f aca="false">maxifs(D$4:D$13,E$4:E$13,"&gt;="&amp;G10)</f>
         <v>#NAME?</v>
       </c>
@@ -3295,19 +3354,19 @@
         <v>0</v>
       </c>
       <c r="C11" s="4"/>
-      <c r="D11" s="5" t="n">
+      <c r="D11" s="6" t="n">
         <f aca="false">COUNTIF(B$4:B11, "=1")/COUNTA(B$4:B11)</f>
         <v>0.5</v>
       </c>
-      <c r="E11" s="6" t="n">
+      <c r="E11" s="7" t="n">
         <f aca="false">COUNTIF(B$4:B11, "=1")/COUNTIF(B$4:B$13,"=1")</f>
         <v>0.8</v>
       </c>
       <c r="F11" s="4"/>
-      <c r="G11" s="6" t="n">
+      <c r="G11" s="7" t="n">
         <v>0.8</v>
       </c>
-      <c r="H11" s="5" t="e">
+      <c r="H11" s="6" t="e">
         <f aca="false">maxifs(D$4:D$13,E$4:E$13,"&gt;="&amp;G11)</f>
         <v>#NAME?</v>
       </c>
@@ -3320,19 +3379,19 @@
         <v>1</v>
       </c>
       <c r="C12" s="4"/>
-      <c r="D12" s="5" t="n">
+      <c r="D12" s="6" t="n">
         <f aca="false">COUNTIF(B$4:B12, "=1")/COUNTA(B$4:B12)</f>
         <v>0.555555555555556</v>
       </c>
-      <c r="E12" s="6" t="n">
+      <c r="E12" s="7" t="n">
         <f aca="false">COUNTIF(B$4:B12, "=1")/COUNTIF(B$4:B$13,"=1")</f>
         <v>1</v>
       </c>
       <c r="F12" s="4"/>
-      <c r="G12" s="6" t="n">
+      <c r="G12" s="7" t="n">
         <v>0.9</v>
       </c>
-      <c r="H12" s="5" t="e">
+      <c r="H12" s="6" t="e">
         <f aca="false">maxifs(D$4:D$13,E$4:E$13,"&gt;="&amp;G12)</f>
         <v>#NAME?</v>
       </c>
@@ -3345,19 +3404,19 @@
         <v>0</v>
       </c>
       <c r="C13" s="4"/>
-      <c r="D13" s="5" t="n">
+      <c r="D13" s="6" t="n">
         <f aca="false">COUNTIF(B$4:B13, "=1")/COUNTA(B$4:B13)</f>
         <v>0.5</v>
       </c>
-      <c r="E13" s="6" t="n">
+      <c r="E13" s="7" t="n">
         <f aca="false">COUNTIF(B$4:B13, "=1")/COUNTIF(B$4:B$13,"=1")</f>
         <v>1</v>
       </c>
       <c r="F13" s="4"/>
-      <c r="G13" s="6" t="n">
-        <v>1</v>
-      </c>
-      <c r="H13" s="5" t="e">
+      <c r="G13" s="7" t="n">
+        <v>1</v>
+      </c>
+      <c r="H13" s="6" t="e">
         <f aca="false">maxifs(D$4:D$13,E$4:E$13,"&gt;="&amp;G13)</f>
         <v>#NAME?</v>
       </c>

</xml_diff>